<commit_message>
Update results and utils
</commit_message>
<xml_diff>
--- a/task_progress/tables/6.4.4tables/table10_hyper_shift.xlsx
+++ b/task_progress/tables/6.4.4tables/table10_hyper_shift.xlsx
@@ -578,65 +578,45 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>0-5</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="F3" t="n">
-        <v>-8</v>
+        <v>-16</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.5</v>
+        <v>-2.5</v>
       </c>
       <c r="H3" t="n">
         <v>-3</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.5</v>
+        <v>-12</v>
       </c>
       <c r="J3" t="n">
         <v>-10</v>
       </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.065</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.155</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-0.735</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-0.175</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>-0.445</v>
-      </c>
-      <c r="R3" t="n">
-        <v>-0.455</v>
-      </c>
-      <c r="S3" t="n">
-        <v>-0.38</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
         <v>0</v>
       </c>
@@ -666,65 +646,45 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>10-15</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-11</v>
+        <v>-7.5</v>
       </c>
       <c r="D4" t="n">
         <v>-4</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.5</v>
+        <v>-4.5</v>
       </c>
       <c r="F4" t="n">
-        <v>-11</v>
+        <v>-17</v>
       </c>
       <c r="G4" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="H4" t="n">
-        <v>-8</v>
+        <v>-7.5</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.5</v>
+        <v>-2</v>
       </c>
       <c r="J4" t="n">
-        <v>-13.5</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-0.155</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.01</v>
-      </c>
+        <v>-8.5</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="n">
         <v>0</v>
       </c>
@@ -754,65 +714,45 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>15-25</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-11</v>
+        <v>-13.5</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5</v>
+        <v>-9</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.5</v>
+        <v>-10</v>
       </c>
       <c r="F5" t="n">
-        <v>-12</v>
+        <v>-21</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="H5" t="n">
-        <v>-5</v>
+        <v>-10.5</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="J5" t="n">
-        <v>-5</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-0.04</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="R5" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.02</v>
-      </c>
+        <v>-14</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
         <v>0</v>
       </c>
@@ -842,65 +782,45 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>25-30</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
+        <v>-13</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E6" t="n">
         <v>-6</v>
       </c>
-      <c r="D6" t="n">
-        <v>-3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-2.5</v>
-      </c>
       <c r="F6" t="n">
+        <v>-19</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-16</v>
+      </c>
+      <c r="I6" t="n">
         <v>-12</v>
       </c>
-      <c r="G6" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-4.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>5</v>
-      </c>
       <c r="J6" t="n">
-        <v>-5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="N6" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="P6" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>-0.135</v>
-      </c>
-      <c r="R6" t="n">
-        <v>-0.555</v>
-      </c>
-      <c r="S6" t="n">
-        <v>-0.04</v>
-      </c>
+        <v>-15</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
         <v>0</v>
       </c>
@@ -930,65 +850,45 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>5-10</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-3</v>
+        <v>-14.5</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F7" t="n">
-        <v>-9</v>
+        <v>-16.5</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.5</v>
+        <v>-2</v>
       </c>
       <c r="H7" t="n">
-        <v>-5</v>
+        <v>-15.5</v>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>-8</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="N7" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="R7" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="S7" t="n">
-        <v>-0.01</v>
-      </c>
+        <v>-15.5</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
         <v>0</v>
       </c>
@@ -1018,65 +918,45 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>≥30</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-4</v>
+        <v>-20</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.5</v>
+        <v>-5</v>
       </c>
       <c r="E8" t="n">
+        <v>-13</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-20</v>
+      </c>
+      <c r="G8" t="n">
         <v>-1</v>
       </c>
-      <c r="F8" t="n">
-        <v>-11.5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2.5</v>
-      </c>
       <c r="H8" t="n">
-        <v>-4</v>
+        <v>-19</v>
       </c>
       <c r="I8" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
-        <v>-4</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.105</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-0.48</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-0.615</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.105</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.08500000000000001</v>
-      </c>
-      <c r="S8" t="n">
-        <v>-0.175</v>
-      </c>
+        <v>-19</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
         <v>0</v>
       </c>

</xml_diff>